<commit_message>
dodanie wierszy na poczatek
</commit_message>
<xml_diff>
--- a/Modele/Przyklad.xlsx
+++ b/Modele/Przyklad.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matek\PycharmProjects\MultiMeasure\Zapis_Wynikow_Wzorcowania\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matek\PycharmProjects\MultiMeasure\Modele\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF1FFACE-FD4F-4831-89F1-F8F74768FB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72242C74-6A13-4592-9A1A-647A52CD1CA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{54C3C7A6-8398-450B-85EA-BA03C00DC2AD}"/>
+    <workbookView xWindow="31365" yWindow="1155" windowWidth="21600" windowHeight="11385" xr2:uid="{54C3C7A6-8398-450B-85EA-BA03C00DC2AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -463,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA7FF516-A456-410C-9AA5-9D8B1E3A4B79}">
-  <dimension ref="B5:F27"/>
+  <dimension ref="B15:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,355 +478,355 @@
     <col min="6" max="6" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1" t="s">
+    <row r="15" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="2">
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="2">
         <v>600</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C17" s="2">
         <v>60</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D17" s="2">
         <v>60</v>
       </c>
-      <c r="E7" s="2">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2">
+      <c r="E17" s="2">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2">
         <v>0.2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2">
-        <v>360</v>
-      </c>
-      <c r="D8" s="2">
-        <v>359.9</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2">
-        <v>540</v>
-      </c>
-      <c r="D9" s="2">
-        <v>539.9</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
-      <c r="C10" s="2">
-        <v>-540</v>
-      </c>
-      <c r="D10" s="2">
-        <v>-539.20000000000005</v>
-      </c>
-      <c r="E10" s="2">
-        <v>-0.8</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="5"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="2">
-        <v>6</v>
-      </c>
-      <c r="C12" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="E12" s="2">
-        <v>0</v>
-      </c>
-      <c r="F12" s="2">
-        <v>2E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2">
-        <v>3.6</v>
-      </c>
-      <c r="D13" s="2">
-        <v>3.6</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0</v>
-      </c>
-      <c r="F13" s="2">
-        <v>2E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
-      <c r="C14" s="2">
-        <v>5.4</v>
-      </c>
-      <c r="D14" s="2">
-        <v>5.399</v>
-      </c>
-      <c r="E14" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="F14" s="2">
-        <v>2E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
-      <c r="C15" s="2">
-        <v>-5.4</v>
-      </c>
-      <c r="D15" s="2">
-        <v>-5.399</v>
-      </c>
-      <c r="E15" s="2">
-        <v>-1E-3</v>
-      </c>
-      <c r="F15" s="2">
-        <v>2E-3</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="2">
-        <v>60</v>
-      </c>
-      <c r="C16" s="2">
-        <v>6</v>
-      </c>
-      <c r="D16" s="2">
-        <v>6</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0</v>
-      </c>
-      <c r="F16" s="2">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="2"/>
-      <c r="C17" s="2">
-        <v>36</v>
-      </c>
-      <c r="D17" s="2">
-        <v>36</v>
-      </c>
-      <c r="E17" s="2">
-        <v>0</v>
-      </c>
-      <c r="F17" s="2">
-        <v>0.02</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2">
-        <v>54</v>
+        <v>360</v>
       </c>
       <c r="D18" s="2">
-        <v>53.99</v>
+        <v>359.9</v>
       </c>
       <c r="E18" s="2">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="F18" s="2">
-        <v>0.02</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2">
-        <v>-54</v>
+        <v>540</v>
       </c>
       <c r="D19" s="2">
-        <v>-54</v>
+        <v>539.9</v>
       </c>
       <c r="E19" s="2">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F19" s="2">
-        <v>0.02</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="2">
-        <v>600</v>
-      </c>
+      <c r="B20" s="2"/>
       <c r="C20" s="2">
-        <v>60</v>
+        <v>-540</v>
       </c>
       <c r="D20" s="2">
-        <v>60</v>
+        <v>-539.20000000000005</v>
       </c>
       <c r="E20" s="2">
-        <v>0</v>
+        <v>-0.8</v>
       </c>
       <c r="F20" s="2">
         <v>0.2</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="2"/>
-      <c r="C21" s="2">
-        <v>360</v>
-      </c>
-      <c r="D21" s="2">
-        <v>360</v>
-      </c>
-      <c r="E21" s="2">
-        <v>0</v>
-      </c>
-      <c r="F21" s="2">
-        <v>0.2</v>
-      </c>
+      <c r="B21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="5"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="2"/>
+      <c r="B22" s="2">
+        <v>6</v>
+      </c>
       <c r="C22" s="2">
-        <v>540</v>
+        <v>0.6</v>
       </c>
       <c r="D22" s="2">
-        <v>540</v>
+        <v>0.6</v>
       </c>
       <c r="E22" s="2">
         <v>0</v>
       </c>
       <c r="F22" s="2">
-        <v>0.2</v>
+        <v>2E-3</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2">
-        <v>-540</v>
+        <v>3.6</v>
       </c>
       <c r="D23" s="2">
-        <v>-540</v>
+        <v>3.6</v>
       </c>
       <c r="E23" s="2">
         <v>0</v>
       </c>
       <c r="F23" s="2">
-        <v>0.2</v>
+        <v>2E-3</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="2">
-        <v>1000</v>
-      </c>
+      <c r="B24" s="2"/>
       <c r="C24" s="2">
-        <v>100</v>
+        <v>5.4</v>
       </c>
       <c r="D24" s="2">
-        <v>100</v>
+        <v>5.399</v>
       </c>
       <c r="E24" s="2">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="F24" s="2">
-        <v>1</v>
+        <v>2E-3</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2">
-        <v>600</v>
+        <v>-5.4</v>
       </c>
       <c r="D25" s="2">
-        <v>600</v>
+        <v>-5.399</v>
       </c>
       <c r="E25" s="2">
-        <v>0</v>
+        <v>-1E-3</v>
       </c>
       <c r="F25" s="2">
-        <v>1</v>
+        <v>2E-3</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="2"/>
+      <c r="B26" s="2">
+        <v>60</v>
+      </c>
       <c r="C26" s="2">
-        <v>900</v>
+        <v>6</v>
       </c>
       <c r="D26" s="2">
-        <v>900</v>
+        <v>6</v>
       </c>
       <c r="E26" s="2">
         <v>0</v>
       </c>
       <c r="F26" s="2">
-        <v>1</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="2">
+        <v>36</v>
+      </c>
+      <c r="D27" s="2">
+        <v>36</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="2"/>
+      <c r="C28" s="2">
+        <v>54</v>
+      </c>
+      <c r="D28" s="2">
+        <v>53.99</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2">
+        <v>-54</v>
+      </c>
+      <c r="D29" s="2">
+        <v>-54</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="2">
+        <v>600</v>
+      </c>
+      <c r="C30" s="2">
+        <v>60</v>
+      </c>
+      <c r="D30" s="2">
+        <v>60</v>
+      </c>
+      <c r="E30" s="2">
+        <v>0</v>
+      </c>
+      <c r="F30" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="2"/>
+      <c r="C31" s="2">
+        <v>360</v>
+      </c>
+      <c r="D31" s="2">
+        <v>360</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="2"/>
+      <c r="C32" s="2">
+        <v>540</v>
+      </c>
+      <c r="D32" s="2">
+        <v>540</v>
+      </c>
+      <c r="E32" s="2">
+        <v>0</v>
+      </c>
+      <c r="F32" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="2"/>
+      <c r="C33" s="2">
+        <v>-540</v>
+      </c>
+      <c r="D33" s="2">
+        <v>-540</v>
+      </c>
+      <c r="E33" s="2">
+        <v>0</v>
+      </c>
+      <c r="F33" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="2">
+        <v>1000</v>
+      </c>
+      <c r="C34" s="2">
+        <v>100</v>
+      </c>
+      <c r="D34" s="2">
+        <v>100</v>
+      </c>
+      <c r="E34" s="2">
+        <v>0</v>
+      </c>
+      <c r="F34" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="2"/>
+      <c r="C35" s="2">
+        <v>600</v>
+      </c>
+      <c r="D35" s="2">
+        <v>600</v>
+      </c>
+      <c r="E35" s="2">
+        <v>0</v>
+      </c>
+      <c r="F35" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="2"/>
+      <c r="C36" s="2">
+        <v>900</v>
+      </c>
+      <c r="D36" s="2">
+        <v>900</v>
+      </c>
+      <c r="E36" s="2">
+        <v>0</v>
+      </c>
+      <c r="F36" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="2"/>
+      <c r="C37" s="2">
         <v>-900</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D37" s="2">
         <v>-900</v>
       </c>
-      <c r="E27" s="2">
-        <v>0</v>
-      </c>
-      <c r="F27" s="2">
+      <c r="E37" s="2">
+        <v>0</v>
+      </c>
+      <c r="F37" s="2">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B21:F21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>